<commit_message>
Stage-2 add A7-A20 tasks
</commit_message>
<xml_diff>
--- a/LevVlad/evidence.xlsx
+++ b/LevVlad/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\CRYPTO FAMILY\NODES\Game NFT\5. Gera.team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\CRYPTO FAMILY\NODES\Game NFT\#5. Gera.team\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="85">
   <si>
     <t>TxHash</t>
   </si>
@@ -70,12 +70,6 @@
   </si>
   <si>
     <t>NFTID</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
   </si>
   <si>
     <t>TeamName</t>
@@ -176,6 +170,135 @@
   <si>
     <t xml:space="preserve">elgafar-1 
 </t>
+  </si>
+  <si>
+    <t>ibc/97404CFF5BD59D79C3A06393A503055C25276B7BD89D86E4ABAD72D55A37A6F6</t>
+  </si>
+  <si>
+    <t>beautiful0007</t>
+  </si>
+  <si>
+    <t>ibc/0FD8267843A0977C0E21B524AD26DFD727C073AF232C1D297F1DD2BD0077D77B</t>
+  </si>
+  <si>
+    <t>beautiful0008</t>
+  </si>
+  <si>
+    <t>ibc/2F0577BD66BDDC806C786218BC7F4F12C63B373A0500643050974D245BBF3E24</t>
+  </si>
+  <si>
+    <t>beautiful0009</t>
+  </si>
+  <si>
+    <t>ibc/3A56031328284E26862F2ABCE068468C31B46FE50D82F6F3FF27A0884D7BC0E</t>
+  </si>
+  <si>
+    <t>beautiful00010</t>
+  </si>
+  <si>
+    <t>ibc/FDD48B4AF972FD7054B63671046FDCB0A9C16405B3A749586BD1485B1DA8EAC8</t>
+  </si>
+  <si>
+    <t>beautiful00011</t>
+  </si>
+  <si>
+    <t>ibc/2055FA438F9AE42CCFA145A4F5B80A3C37E8C002E801EAD8716162EA1B431861</t>
+  </si>
+  <si>
+    <t>beautiful00012</t>
+  </si>
+  <si>
+    <t>509076DE9646B3FA4A99DDF0035DD7A5BED3BB4B3222A825CD34D4658D895DD5</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>BCBE1D667C2C41B07DE293E5FD51118F95EFEAC84D0B1081DB2331C3A185DD05</t>
+  </si>
+  <si>
+    <t>048648871B9F8F833B6FB92ADCE27D7D4E7580DDB1F2C5B57D4148358886C405</t>
+  </si>
+  <si>
+    <t>8D415C14E13912AF4AC0603EAC13CEE45575673B21FCB6F36542E9C7EE270FF0</t>
+  </si>
+  <si>
+    <t>3C52B382B401CDC07B1FCA0A9EAB4A64C4470E0A12F0E77CF3F1D78659F227E6</t>
+  </si>
+  <si>
+    <t>7693FA869957AE52CB9186B71BEA56ED786E711C46744CDD667CB622FE0C7E05</t>
+  </si>
+  <si>
+    <t>188D1702A9E5A81E63279910C02794361D740CC9D55001A45A0DE77B8D550565</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>E6852A02D3761EE34E0D8EBA7619B5E73C0161C0CD9460575B9134C6A50533CE</t>
+  </si>
+  <si>
+    <t>86D7DC7125063610EC0C7745E3556E96AC24D430934A2674CCBFBD42466B8E55</t>
+  </si>
+  <si>
+    <t>31188FABE49A57DEF7F4DA8693AFF0735BDA144320E78E0BFEBF786982D7425C</t>
+  </si>
+  <si>
+    <t>2033D5284354A757C7EBA395851114359DB75E8F1CCB990E3A88B8287C56CB0C</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>982D6F1C6874CBF51F939EF3043057EBE9E04A7AA20B537EC6157ED8B9CF0FA5</t>
+  </si>
+  <si>
+    <t>8F727C8D89861F61026747308E1B7DDF8BE9F61718CA618DA355688766041091</t>
+  </si>
+  <si>
+    <t>2B4C2138FECFD7142F67044185CBBA5D95BC5EA17BD8E27F5BF6D6B1F1262D3F</t>
+  </si>
+  <si>
+    <t>D78566673CFCDE38FBFC9E515761541040600AEDDADEB9030DF7B76BF19766B5</t>
+  </si>
+  <si>
+    <t>D718270EC9740D2734B8626C4E87B85657142EFFF40EA1C9075AF0D7ADE62F1A</t>
+  </si>
+  <si>
+    <t>B26C72FC1AACB784AFEF1F2CA5DE63C7D077E3D51D45C352A89366F28BBEE2EA</t>
+  </si>
+  <si>
+    <t>9BE33236FBD3D317EC7D7557082ACA6489FD7F190D3105787E74885C95C293CA</t>
+  </si>
+  <si>
+    <t>8B0E00ACC9A04F522A6EBA5ADAF3D8C5334452F82B3BA9DE974CCD2A787EF937</t>
+  </si>
+  <si>
+    <t>94D59677EBC400AC0AD45A7DDDC65ADC8B8494DF25FF5428ED9D4BCE05F6DD99</t>
+  </si>
+  <si>
+    <t>A01D420B950F34EBFCA6C4F3FA147B087F355E14367CA75E7C996EC85E764271</t>
+  </si>
+  <si>
+    <t>1824F97FF89C0DA13CB79ABD19D837F090917855242B5D6D56890D5DF32286B6</t>
+  </si>
+  <si>
+    <t>95AB0D450EAA33178EEEFB78ABAAF17CEB5DA2B3DB6890E91DE2EDDC4C65EE78</t>
+  </si>
+  <si>
+    <t>8F24251521CE967B1FA0C9BE1E216329395AD63F3B485AF79D75F5A035A4DB44</t>
+  </si>
+  <si>
+    <t>A4E7EEAB6918B68A6867C9700D24BFA5EA4CC53A0633337C447A1F4159DDD358</t>
+  </si>
+  <si>
+    <t>392E6482BE51A2DA4FBBDDB653A237CEE766B2108432D41C09719DFA406DDB18</t>
+  </si>
+  <si>
+    <t>28A65292477B8840C0C2136E91D6428AB4A4C059C55009FB97FE29146637C954</t>
+  </si>
+  <si>
+    <t>4CD4045F4FF8C61610B707C3F0E7ECDE91B6D842481EE5F2F8E58749D6B1A72F</t>
   </si>
 </sst>
 </file>
@@ -590,54 +713,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -652,7 +775,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -670,10 +795,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -688,7 +813,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -706,10 +833,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +851,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -742,10 +871,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -760,7 +889,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -768,7 +899,7 @@
     <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -778,10 +909,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -794,9 +925,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -814,23 +947,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -842,9 +987,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -862,23 +1009,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -986,9 +1145,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1006,23 +1167,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1034,9 +1207,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1054,23 +1229,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1103,10 +1290,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1120,9 +1307,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1140,23 +1329,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1168,9 +1385,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1188,23 +1407,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1377,35 +1624,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1447,16 +1694,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1498,16 +1745,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1549,16 +1796,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1601,16 +1848,16 @@
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -18005,7 +18252,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18023,14 +18272,15 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18041,7 +18291,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18059,10 +18311,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new task add Stage-2
</commit_message>
<xml_diff>
--- a/LevVlad/evidence.xlsx
+++ b/LevVlad/evidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10605" firstSheet="4" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="90">
   <si>
     <t>TxHash</t>
   </si>
@@ -55,15 +55,6 @@
   </si>
   <si>
     <t>ChainID</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
   </si>
   <si>
     <t>ClassID</t>
@@ -299,6 +290,30 @@
   </si>
   <si>
     <t>4CD4045F4FF8C61610B707C3F0E7ECDE91B6D842481EE5F2F8E58749D6B1A72F</t>
+  </si>
+  <si>
+    <t>7DD176636F1DE5D0F9B90E08C7567A2D80143EE35B4E64C02413BEE9AEB3A011</t>
+  </si>
+  <si>
+    <t>C0B2AA797136C28F357C5725CC88DEEB2884E4EC361233E02D03DD97CE634EA7</t>
+  </si>
+  <si>
+    <t>AFD1113BC24F5E247F1177D504F497CEB5162B56A41E4FFF55F06E32E4D880B9</t>
+  </si>
+  <si>
+    <t>531182B81FADFF2AA14EF45B8DB4216CFC2C97F5593262A75E76CFCD8D002388</t>
+  </si>
+  <si>
+    <t>A0B6A0F8566491E5B5F6E2D5F4BF76F4742CA62BE1611449898E562C9E0F27A7</t>
+  </si>
+  <si>
+    <t>F4E4FE7FE0B0B894B3C92D0C90E2122CA2C609510928E078EA5302876B2CA69C</t>
+  </si>
+  <si>
+    <t>F8A86BF1E074075A7C4BCDA74D7AA52DC2E697FA51C0F366CCEF58A3B1F5A840</t>
+  </si>
+  <si>
+    <t>FD583813531B278D8DE86AF749FD77808751B2E04FB7A0E65C51259C4909DB22</t>
   </si>
 </sst>
 </file>
@@ -695,7 +710,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -713,54 +728,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -787,18 +802,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -825,18 +840,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -863,18 +878,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -901,18 +916,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -947,34 +962,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1009,34 +1024,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1049,9 +1064,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1069,26 +1086,39 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1097,9 +1127,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1117,23 +1149,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1167,34 +1211,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1229,34 +1273,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1285,15 +1329,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1329,50 +1373,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1407,50 +1451,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1616,43 +1660,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1683,10 +1727,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1694,16 +1738,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1734,10 +1778,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1745,16 +1789,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1785,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1796,16 +1840,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1837,10 +1881,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1848,16 +1892,16 @@
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -18264,18 +18308,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -18303,18 +18347,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>